<commit_message>
Avanzando en la documentacion. 80% diagramas de actividad hechos
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
+++ b/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
   <si>
     <t>EDICIÓN DE PACIENTE</t>
   </si>
   <si>
-    <t>LISTADO DE VÍDEOS ASOCIADOS A EXPLORACIÓN</t>
-  </si>
-  <si>
     <t>LISTADO DE GRÁFICAS (FICHEROS EMT) ASOCIADOS A EXPLORACIÓN</t>
   </si>
   <si>
@@ -36,9 +33,6 @@
     <t>ALTA DE USUARIOS</t>
   </si>
   <si>
-    <t>EDICIÓN DE USUARIOS</t>
-  </si>
-  <si>
     <t>ELIMINACIÓN DE USUARIOS</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t>ACT-10</t>
   </si>
   <si>
-    <t>in work</t>
-  </si>
-  <si>
     <t>ACT-11</t>
   </si>
   <si>
@@ -247,6 +238,39 @@
   </si>
   <si>
     <t>ACT-14</t>
+  </si>
+  <si>
+    <t>ACT15</t>
+  </si>
+  <si>
+    <t>ACT16</t>
+  </si>
+  <si>
+    <t>LISTADO DE VÍDEOS</t>
+  </si>
+  <si>
+    <t>ACT-17</t>
+  </si>
+  <si>
+    <t>ACT-18</t>
+  </si>
+  <si>
+    <t>ACT-19</t>
+  </si>
+  <si>
+    <t>ACT-21</t>
+  </si>
+  <si>
+    <t>ACT-22</t>
+  </si>
+  <si>
+    <t>EDITAR USUARIO</t>
+  </si>
+  <si>
+    <t>ACT-23</t>
+  </si>
+  <si>
+    <t>ACT-24</t>
   </si>
 </sst>
 </file>
@@ -297,12 +321,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -337,6 +355,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -351,28 +375,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -384,11 +405,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -702,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,567 +746,585 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="13"/>
+      <c r="A1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>15</v>
+        <v>54</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>54</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>13</v>
+        <v>54</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>9</v>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>9</v>
+      <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>20</v>
+        <v>54</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>39</v>
+        <v>54</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>9</v>
+      <c r="D9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>54</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>58</v>
+        <v>22</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>22</v>
+        <v>54</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>26</v>
+        <v>54</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>40</v>
+        <v>54</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>30</v>
+        <v>54</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="5" t="s">
-        <v>58</v>
+        <v>76</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>33</v>
+        <v>54</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>72</v>
+        <v>30</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>34</v>
+        <v>54</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>72</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>35</v>
+        <v>54</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>72</v>
+        <v>27</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>36</v>
+        <v>54</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="5" t="s">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>37</v>
+        <v>54</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="5" t="s">
-        <v>58</v>
+        <v>2</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>41</v>
+        <v>55</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="5" t="s">
-        <v>58</v>
+        <v>3</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="5" t="s">
-        <v>58</v>
+        <v>40</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="5" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="5" t="s">
-        <v>58</v>
+        <v>4</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="5" t="s">
-        <v>58</v>
+        <v>82</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>48</v>
+        <v>55</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="5" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="5" t="s">
-        <v>58</v>
+        <v>6</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="5" t="s">
-        <v>58</v>
+      <c r="C30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plantilla analisis del sistema con diagrama contextual del sistema
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
+++ b/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
   <si>
     <t>EDICIÓN DE PACIENTE</t>
   </si>
@@ -36,9 +36,6 @@
     <t>ELIMINACIÓN DE USUARIOS</t>
   </si>
   <si>
-    <t>SUBIDA DE FICHEROS EMT ASOCIADOS A EXPLORACIONES DE PACIENTES</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -271,6 +268,21 @@
   </si>
   <si>
     <t>ACT-24</t>
+  </si>
+  <si>
+    <t>SUBIR FICHEROS EMT</t>
+  </si>
+  <si>
+    <t>ACT-25</t>
+  </si>
+  <si>
+    <t>ACT-26</t>
+  </si>
+  <si>
+    <t>ACT-27</t>
+  </si>
+  <si>
+    <t>ACT-28</t>
   </si>
 </sst>
 </file>
@@ -307,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,12 +367,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -375,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -405,20 +411,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -732,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,375 +745,375 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1122,209 +1121,217 @@
         <v>54</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="5" t="s">
-        <v>56</v>
+        <v>3</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>78</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>79</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>80</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>81</v>
+        <v>6</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>83</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="13" t="s">
-        <v>56</v>
+        <v>6</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>17</v>
-      </c>
       <c r="D28" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="14" t="s">
-        <v>56</v>
+        <v>6</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>49</v>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="14" t="s">
-        <v>56</v>
+        <v>6</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="14" t="s">
-        <v>56</v>
+      <c r="E30" s="11"/>
+      <c r="F30" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
He retocado documentos: - Mejora en general -Añadir casos de uso de faqs - Imagenes del project - Coste del proyecto
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
+++ b/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
   <si>
     <t>EDICIÓN DE PACIENTE</t>
   </si>
@@ -216,9 +216,6 @@
     <t>ACT-08</t>
   </si>
   <si>
-    <t>FAQS</t>
-  </si>
-  <si>
     <t>ACT-09</t>
   </si>
   <si>
@@ -283,6 +280,45 @@
   </si>
   <si>
     <t>ACT-28</t>
+  </si>
+  <si>
+    <t>VISUALIZAR FAQS</t>
+  </si>
+  <si>
+    <t>CDU-29</t>
+  </si>
+  <si>
+    <t>DETALLE FAQS</t>
+  </si>
+  <si>
+    <t>ALTA FAQS</t>
+  </si>
+  <si>
+    <t>EDITAR FAQS</t>
+  </si>
+  <si>
+    <t>BORRAR FAQS</t>
+  </si>
+  <si>
+    <t>SUGERIR FAQS</t>
+  </si>
+  <si>
+    <t>CDU-30</t>
+  </si>
+  <si>
+    <t>CDU-31</t>
+  </si>
+  <si>
+    <t>CDU-32</t>
+  </si>
+  <si>
+    <t>CDU-33</t>
+  </si>
+  <si>
+    <t>CDU-34</t>
+  </si>
+  <si>
+    <t>APROBAR SUGERENCIAS FAQS</t>
   </si>
 </sst>
 </file>
@@ -729,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>6</v>
@@ -970,7 +1006,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>6</v>
@@ -990,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>6</v>
@@ -1004,13 +1040,13 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>6</v>
@@ -1030,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>6</v>
@@ -1050,7 +1086,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>6</v>
@@ -1070,7 +1106,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>6</v>
@@ -1090,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>6</v>
@@ -1110,7 +1146,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>6</v>
@@ -1130,7 +1166,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>6</v>
@@ -1150,7 +1186,7 @@
         <v>6</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>6</v>
@@ -1170,7 +1206,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>6</v>
@@ -1190,7 +1226,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>6</v>
@@ -1204,13 +1240,13 @@
         <v>44</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>82</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>6</v>
@@ -1230,7 +1266,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>6</v>
@@ -1244,13 +1280,13 @@
         <v>46</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>85</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>6</v>
@@ -1270,7 +1306,7 @@
         <v>6</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>6</v>
@@ -1290,7 +1326,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>6</v>
@@ -1310,7 +1346,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>6</v>
@@ -1324,13 +1360,112 @@
         <v>35</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>55</v>
+        <v>88</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mejora de los documentos del 01-04 (de acuerdo al nuevo libro facilitado por el profesor que esta bastante bien)
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
+++ b/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
@@ -355,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +403,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -417,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,6 +462,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
@@ -767,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +826,7 @@
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -839,7 +846,7 @@
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -859,7 +866,7 @@
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -879,7 +886,7 @@
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -899,7 +906,7 @@
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -919,7 +926,7 @@
       <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -939,7 +946,7 @@
       <c r="B9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -959,7 +966,7 @@
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -979,7 +986,7 @@
       <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -999,7 +1006,7 @@
       <c r="B12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -1019,7 +1026,7 @@
       <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1039,7 +1046,7 @@
       <c r="B14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -1059,7 +1066,7 @@
       <c r="B15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -1079,7 +1086,7 @@
       <c r="B16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="14" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1099,7 +1106,7 @@
       <c r="B17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1119,7 +1126,7 @@
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1139,7 +1146,7 @@
       <c r="B19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1159,7 +1166,7 @@
       <c r="B20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -1179,7 +1186,7 @@
       <c r="B21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -1199,7 +1206,7 @@
       <c r="B22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -1219,7 +1226,7 @@
       <c r="B23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="14" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -1239,7 +1246,7 @@
       <c r="B24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="14" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -1259,7 +1266,7 @@
       <c r="B25" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -1279,7 +1286,7 @@
       <c r="B26" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -1299,7 +1306,7 @@
       <c r="B27" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -1319,7 +1326,7 @@
       <c r="B28" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -1339,7 +1346,7 @@
       <c r="B29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="7" t="s">

</xml_diff>

<commit_message>
documentacion: d.clases y secuencia actas
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
+++ b/documentacion/Documentacion_final/Utiles/estado de los casos de uso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="112">
   <si>
     <t>EDICIÓN DE PACIENTE</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>ACT-36</t>
+  </si>
+  <si>
+    <t>D. CLASES</t>
+  </si>
+  <si>
+    <t>PENDING</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -474,6 +480,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,21 +821,25 @@
     <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="16"/>
+      <c r="G1" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -835,8 +858,11 @@
       <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -855,8 +881,11 @@
       <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
@@ -875,8 +904,11 @@
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -895,8 +927,11 @@
       <c r="F5" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -915,8 +950,11 @@
       <c r="F6" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -935,8 +973,11 @@
       <c r="F7" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -955,8 +996,11 @@
       <c r="F8" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -975,8 +1019,11 @@
       <c r="F9" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -995,8 +1042,11 @@
       <c r="F10" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -1015,28 +1065,34 @@
       <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="G11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -1055,8 +1111,11 @@
       <c r="F13" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -1075,8 +1134,11 @@
       <c r="F14" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
@@ -1095,8 +1157,11 @@
       <c r="F15" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -1115,8 +1180,11 @@
       <c r="F16" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1135,8 +1203,11 @@
       <c r="F17" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -1155,8 +1226,11 @@
       <c r="F18" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -1175,28 +1249,34 @@
       <c r="F19" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="G19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="D20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
@@ -1215,8 +1295,11 @@
       <c r="F21" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1235,8 +1318,11 @@
       <c r="F22" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -1255,8 +1341,11 @@
       <c r="F23" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -1275,8 +1364,11 @@
       <c r="F24" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -1295,28 +1387,34 @@
       <c r="F25" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="G25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="D26" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -1335,8 +1433,11 @@
       <c r="F27" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -1355,8 +1456,11 @@
       <c r="F28" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -1375,8 +1479,11 @@
       <c r="F29" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1395,28 +1502,34 @@
       <c r="F30" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="G30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="13" t="s">
         <v>87</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="9" t="s">
+      <c r="D31" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -1435,8 +1548,11 @@
       <c r="F32" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -1455,8 +1571,11 @@
       <c r="F33" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
@@ -1475,8 +1594,11 @@
       <c r="F34" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
@@ -1495,8 +1617,11 @@
       <c r="F35" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1515,8 +1640,11 @@
       <c r="F36" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
@@ -1534,6 +1662,9 @@
       </c>
       <c r="F37" s="5" t="s">
         <v>6</v>
+      </c>
+      <c r="G37" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>